<commit_message>
Finalized PRF and Templates
</commit_message>
<xml_diff>
--- a/REMITTANCE_PRF.xlsx
+++ b/REMITTANCE_PRF.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PROGRAMMING\Python\Excel_Project\excel_proj\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PROGRAMMING\Python\excelProj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BD2DECA-9558-451B-8396-98905C4B6ACA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26F02C36-3341-4053-A8DE-F0D4A8D00886}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="REMIT" sheetId="1" r:id="rId1"/>
@@ -558,21 +558,21 @@
   <dimension ref="A1:M50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="6" max="6" width="15.88671875" customWidth="1"/>
-    <col min="9" max="9" width="17.109375" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" customWidth="1"/>
     <col min="10" max="10" width="17" customWidth="1"/>
-    <col min="11" max="11" width="17.88671875" customWidth="1"/>
-    <col min="12" max="12" width="14.5546875" customWidth="1"/>
-    <col min="13" max="13" width="19.6640625" customWidth="1"/>
+    <col min="11" max="11" width="17.85546875" customWidth="1"/>
+    <col min="12" max="12" width="14.5703125" customWidth="1"/>
+    <col min="13" max="13" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -613,7 +613,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -650,7 +650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -659,7 +659,7 @@
       <c r="D3" s="8"/>
       <c r="E3" s="17"/>
       <c r="F3" s="18">
-        <f t="shared" ref="F2:F17" si="6">24.7%*E3</f>
+        <f t="shared" ref="F3:F17" si="6">24.7%*E3</f>
         <v>0</v>
       </c>
       <c r="G3" s="18">
@@ -690,7 +690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -730,7 +730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -770,7 +770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -810,7 +810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -850,7 +850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -890,7 +890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -924,7 +924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -964,7 +964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -1004,7 +1004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -1044,7 +1044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -1084,7 +1084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -1124,7 +1124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -1164,7 +1164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -1204,7 +1204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -1244,7 +1244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -1275,7 +1275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -1315,7 +1315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -1355,7 +1355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -1395,7 +1395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -1435,7 +1435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -1475,7 +1475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -1515,7 +1515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>24</v>
       </c>
@@ -1555,7 +1555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -1595,7 +1595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>26</v>
       </c>
@@ -1635,7 +1635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>27</v>
       </c>
@@ -1675,7 +1675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -1715,7 +1715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>29</v>
       </c>
@@ -1755,7 +1755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -1795,7 +1795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>31</v>
       </c>
@@ -1835,7 +1835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>32</v>
       </c>
@@ -1875,7 +1875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>33</v>
       </c>
@@ -1915,7 +1915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>34</v>
       </c>
@@ -1955,7 +1955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>35</v>
       </c>
@@ -1995,7 +1995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>36</v>
       </c>
@@ -2035,7 +2035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>37</v>
       </c>
@@ -2075,7 +2075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>38</v>
       </c>
@@ -2115,7 +2115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>39</v>
       </c>
@@ -2155,7 +2155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>40</v>
       </c>
@@ -2195,7 +2195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>41</v>
       </c>
@@ -2235,7 +2235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>42</v>
       </c>
@@ -2275,7 +2275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>43</v>
       </c>
@@ -2315,7 +2315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <v>44</v>
       </c>
@@ -2355,7 +2355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <v>45</v>
       </c>
@@ -2395,7 +2395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <v>46</v>
       </c>
@@ -2435,7 +2435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>47</v>
       </c>
@@ -2475,7 +2475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
         <v>48</v>
       </c>
@@ -2515,7 +2515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
         <v>49</v>
       </c>

</xml_diff>